<commit_message>
Sample courses spread sheet with heading
</commit_message>
<xml_diff>
--- a/public/imports/courses/courses.xlsx
+++ b/public/imports/courses/courses.xlsx
@@ -20,42 +20,18 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="12">
-  <si>
-    <t xml:space="preserve">simple course</t>
-  </si>
-  <si>
-    <t xml:space="preserve">imported course</t>
-  </si>
-  <si>
-    <t xml:space="preserve">another course</t>
-  </si>
-  <si>
-    <t xml:space="preserve">just another course</t>
-  </si>
-  <si>
-    <t xml:space="preserve">same thing</t>
-  </si>
-  <si>
-    <t xml:space="preserve">just samething</t>
-  </si>
-  <si>
-    <t xml:space="preserve">testing</t>
-  </si>
-  <si>
-    <t xml:space="preserve">testing again</t>
-  </si>
-  <si>
-    <t xml:space="preserve">it is beautiful</t>
-  </si>
-  <si>
-    <t xml:space="preserve">wooow it is beautiful</t>
-  </si>
-  <si>
-    <t xml:space="preserve">this is added</t>
-  </si>
-  <si>
-    <t xml:space="preserve">added something new</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+  <si>
+    <t xml:space="preserve">Name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Description</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Certificate in Welding</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Certificate in Hair dressing</t>
   </si>
 </sst>
 </file>
@@ -65,7 +41,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="7">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -86,6 +62,21 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="10"/>
+      <color rgb="FF0000FF"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -137,12 +128,20 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -163,88 +162,35 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C7"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C7" activeCellId="0" sqref="C7"/>
+      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="27.78"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="36.84"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="4" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="27.78"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="36.84"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="3" style="0" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="B1" s="1" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="0" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="n">
+      <c r="A2" s="3" t="s">
         <v>2</v>
-      </c>
-      <c r="B2" s="0" t="s">
-        <v>2</v>
-      </c>
-      <c r="C2" s="0" t="s">
-        <v>3</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="B3" s="0" t="s">
-        <v>4</v>
-      </c>
-      <c r="C3" s="0" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="B4" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="C4" s="0" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="B5" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="C5" s="0" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="n">
+      <c r="A3" s="0" t="s">
         <v>3</v>
-      </c>
-      <c r="B6" s="0" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B7" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="C7" s="0" t="s">
-        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>